<commit_message>
month report email working
</commit_message>
<xml_diff>
--- a/savedFiles/TemplateMonthlyReport.xlsx
+++ b/savedFiles/TemplateMonthlyReport.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kthompson.SALEPOINT\Documents\Titans\2014-2015\TimeSubmission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Documents\BYU-I\2020 Winter\CS 499\dues-reduction-app\backend\savedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921576A-C19B-4718-8774-F8112E68DBB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="20625" windowHeight="11370"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TimeEntry" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -26,9 +27,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>PNC Arena - Member Credit Sumary</t>
-  </si>
   <si>
     <t>TU Account</t>
   </si>
@@ -44,12 +42,15 @@
   <si>
     <t>Credit</t>
   </si>
+  <si>
+    <t xml:space="preserve">Dues Reduction Credits for : </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +67,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
@@ -163,8 +172,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -172,6 +199,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF98FB98"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -259,6 +291,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -294,6 +343,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,14 +535,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,48 +559,60 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="13"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="13"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E6" s="13"/>
@@ -554,9 +632,15 @@
     <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E11" s="13"/>
     </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -564,7 +648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>